<commit_message>
EE english version prototype. (other majors are affected, due to changing code)
</commit_message>
<xml_diff>
--- a/database/ElectricalEngineering/EE_Course_database.xlsx
+++ b/database/ElectricalEngineering/EE_Course_database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\20110706\TaiGer_Transcript-Program_Comparer\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\20110706\TaiGer_Transcript-Program_Comparer\database\ElectricalEngineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56983250-4BB1-44A9-B083-C3D2056982D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4733D7FF-7780-49E3-8B0D-49FD8B64F279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21825" yWindow="-16350" windowWidth="29040" windowHeight="15840" xr2:uid="{4A678F9F-A21C-41A5-9AEE-FA5C928DC178}"/>
+    <workbookView xWindow="-6975" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{4A678F9F-A21C-41A5-9AEE-FA5C928DC178}"/>
   </bookViews>
   <sheets>
     <sheet name="All_EE_Courses" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="186">
   <si>
     <t>再生能源導論</t>
   </si>
@@ -84,9 +84,6 @@
     <t>光電子學(一)</t>
   </si>
   <si>
-    <t>資料探勘導論</t>
-  </si>
-  <si>
     <t>進階微波被動電路設計與分析</t>
   </si>
   <si>
@@ -219,9 +216,6 @@
     <t>軟體工程</t>
   </si>
   <si>
-    <t>平行運算</t>
-  </si>
-  <si>
     <t>高頻電路</t>
   </si>
   <si>
@@ -310,13 +304,292 @@
   </si>
   <si>
     <t>超大型積體電路</t>
+  </si>
+  <si>
+    <t>Calculus (1)</t>
+  </si>
+  <si>
+    <t>Calculus (2)</t>
+  </si>
+  <si>
+    <t>Linear algebra</t>
+  </si>
+  <si>
+    <t>Differential equation</t>
+  </si>
+  <si>
+    <t>discrete mathematics</t>
+  </si>
+  <si>
+    <t>Probability and Statistics</t>
+  </si>
+  <si>
+    <t>Numerical Analysis</t>
+  </si>
+  <si>
+    <t>Complex function</t>
+  </si>
+  <si>
+    <t>Modern physics</t>
+  </si>
+  <si>
+    <t>Introduction to Computer</t>
+  </si>
+  <si>
+    <t>Computer organization</t>
+  </si>
+  <si>
+    <t>Computer structure</t>
+  </si>
+  <si>
+    <t>Software engineering</t>
+  </si>
+  <si>
+    <t>Embedded programming</t>
+  </si>
+  <si>
+    <t>Data structure</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t>Object-oriented programming</t>
+  </si>
+  <si>
+    <t>Automatic control (1)</t>
+  </si>
+  <si>
+    <t>Smart control</t>
+  </si>
+  <si>
+    <t>Control System</t>
+  </si>
+  <si>
+    <t>Non-linear control system</t>
+  </si>
+  <si>
+    <t>Electronic Experiment (1)</t>
+  </si>
+  <si>
+    <t>Electronic Experiment (2)</t>
+  </si>
+  <si>
+    <t>Electronics (1)</t>
+  </si>
+  <si>
+    <t>Electronics (2)</t>
+  </si>
+  <si>
+    <t>Electronics (3)</t>
+  </si>
+  <si>
+    <t>Optoelectronics (1)</t>
+  </si>
+  <si>
+    <t>Digital logic</t>
+  </si>
+  <si>
+    <t>Integrated circuit process technology</t>
+  </si>
+  <si>
+    <t>Integrated circuit design</t>
+  </si>
+  <si>
+    <t>Analog integrated circuit design</t>
+  </si>
+  <si>
+    <t>Digital integrated circuit design</t>
+  </si>
+  <si>
+    <t>Advanced microwave passive circuit design and analysis</t>
+  </si>
+  <si>
+    <t>Signal and system</t>
+  </si>
+  <si>
+    <t>Electromagnetism (1)</t>
+  </si>
+  <si>
+    <t>Electromagnetism (2)</t>
+  </si>
+  <si>
+    <t>High frequency circuit</t>
+  </si>
+  <si>
+    <t>Power system planning and operation</t>
+  </si>
+  <si>
+    <t>Semiconductor laser</t>
+  </si>
+  <si>
+    <t>Semiconductor packaging and trend development</t>
+  </si>
+  <si>
+    <t>Component design and model establishment</t>
+  </si>
+  <si>
+    <t>Semiconductor component physics</t>
+  </si>
+  <si>
+    <t>Optoelectronics Physics</t>
+  </si>
+  <si>
+    <t>Communication principle (1)</t>
+  </si>
+  <si>
+    <t>Communication Principle (2)</t>
+  </si>
+  <si>
+    <t>Digital communication</t>
+  </si>
+  <si>
+    <t>Message theory</t>
+  </si>
+  <si>
+    <t>Antenna principle and design</t>
+  </si>
+  <si>
+    <t>Introduction to Renewable Energy</t>
+  </si>
+  <si>
+    <t>Introduction to Power Engineering</t>
+  </si>
+  <si>
+    <t>Introduction to Wireless Networks</t>
+  </si>
+  <si>
+    <t>Computer vision</t>
+  </si>
+  <si>
+    <t>Image processing</t>
+  </si>
+  <si>
+    <t>Internet of Things Technology</t>
+  </si>
+  <si>
+    <t>Cryptography and experiment</t>
+  </si>
+  <si>
+    <t>Green Energy Technology and System</t>
+  </si>
+  <si>
+    <t>On-screen fingerprint recognition in deep learning</t>
+  </si>
+  <si>
+    <t>Vector analysis</t>
+  </si>
+  <si>
+    <t>Photoelectric sensing technology and application</t>
+  </si>
+  <si>
+    <t>Applied Quantum Mechanics (1)</t>
+  </si>
+  <si>
+    <t>Advanced Renewable Energy Implementation Topic</t>
+  </si>
+  <si>
+    <t>Introduction to Medical Engineering</t>
+  </si>
+  <si>
+    <t>Introduction to Microwave Engineering</t>
+  </si>
+  <si>
+    <t>statics</t>
+  </si>
+  <si>
+    <t>dynamics</t>
+  </si>
+  <si>
+    <t>Thermodynamics</t>
+  </si>
+  <si>
+    <t>Fluid mechanics</t>
+  </si>
+  <si>
+    <t>Heat transfer</t>
+  </si>
+  <si>
+    <t>Mobility</t>
+  </si>
+  <si>
+    <t>Communication network</t>
+  </si>
+  <si>
+    <t>Power Electronics</t>
+  </si>
+  <si>
+    <t>Power Systems</t>
+  </si>
+  <si>
+    <t>Bioimaging</t>
+  </si>
+  <si>
+    <t>Electronic components and materials</t>
+  </si>
+  <si>
+    <t>acoustics</t>
+  </si>
+  <si>
+    <t>Data transfer</t>
+  </si>
+  <si>
+    <t>Compiler principle</t>
+  </si>
+  <si>
+    <t>Microsystem manufacturing</t>
+  </si>
+  <si>
+    <t>High frequency system engineering</t>
+  </si>
+  <si>
+    <t>Electric motor</t>
+  </si>
+  <si>
+    <t>Power Electronics Experiment</t>
+  </si>
+  <si>
+    <t>所有科目_英語</t>
+  </si>
+  <si>
+    <t>Electrical Circuits (1)</t>
+  </si>
+  <si>
+    <t>Electrical Circuits (2)</t>
+  </si>
+  <si>
+    <t>Automatic control (2)</t>
+  </si>
+  <si>
+    <t>Operating system</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Physics (1)</t>
+  </si>
+  <si>
+    <t>Physics (2)</t>
+  </si>
+  <si>
+    <t>Physics Experiment (1)</t>
+  </si>
+  <si>
+    <t>Physics Experiment (2)</t>
+  </si>
+  <si>
+    <t>Semiconductor manufacture and measurement</t>
+  </si>
+  <si>
+    <t>Very large Scale integrated circuit (VLSI)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -376,6 +649,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Linux Libertine G"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Linux Libertine G"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -402,7 +686,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -435,6 +719,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -750,23 +1040,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C323114-BC5F-49C1-9F53-9EA9AB7CC060}">
-  <dimension ref="A1:W420"/>
+  <dimension ref="A1:W418"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="21.09765625" style="2" customWidth="1"/>
-    <col min="2" max="16384" width="8.796875" style="2"/>
+    <col min="1" max="1" width="22.69921875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21.19921875" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="4"/>
+        <v>85</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>174</v>
+      </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -791,7 +1084,9 @@
       <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4"/>
+      <c r="B2" s="14" t="s">
+        <v>93</v>
+      </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -814,9 +1109,11 @@
     </row>
     <row r="3" spans="1:23">
       <c r="A3" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>35</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>94</v>
+      </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -839,9 +1136,11 @@
     </row>
     <row r="4" spans="1:23">
       <c r="A4" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>37</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>95</v>
+      </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -864,9 +1163,11 @@
     </row>
     <row r="5" spans="1:23">
       <c r="A5" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" s="5"/>
+        <v>83</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>96</v>
+      </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -889,9 +1190,11 @@
     </row>
     <row r="6" spans="1:23">
       <c r="A6" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>97</v>
+      </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -912,11 +1215,13 @@
       <c r="V6" s="5"/>
       <c r="W6" s="7"/>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" ht="30.6">
       <c r="A7" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>98</v>
+      </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="H7" s="5"/>
@@ -938,9 +1243,11 @@
     </row>
     <row r="8" spans="1:23">
       <c r="A8" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="5"/>
+        <v>42</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>99</v>
+      </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="H8" s="5"/>
@@ -962,9 +1269,11 @@
     </row>
     <row r="9" spans="1:23">
       <c r="A9" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="5"/>
+        <v>41</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>100</v>
+      </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="H9" s="5"/>
@@ -988,7 +1297,9 @@
       <c r="A10" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="14" t="s">
+        <v>180</v>
+      </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="H10" s="5"/>
@@ -1010,9 +1321,11 @@
     </row>
     <row r="11" spans="1:23">
       <c r="A11" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>181</v>
+      </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="H11" s="5"/>
@@ -1032,11 +1345,13 @@
       <c r="V11" s="1"/>
       <c r="W11" s="7"/>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:23" ht="30.6">
       <c r="A12" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="14" t="s">
+        <v>182</v>
+      </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="H12" s="5"/>
@@ -1056,11 +1371,13 @@
       <c r="V12" s="1"/>
       <c r="W12" s="7"/>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:23" ht="30.6">
       <c r="A13" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B13" s="5"/>
+        <v>81</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>183</v>
+      </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="H13" s="5"/>
@@ -1082,9 +1399,11 @@
     </row>
     <row r="14" spans="1:23">
       <c r="A14" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>101</v>
+      </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="H14" s="5"/>
@@ -1104,11 +1423,13 @@
       <c r="V14" s="1"/>
       <c r="W14" s="7"/>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:23" ht="30.6">
       <c r="A15" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="B15" s="5"/>
+        <v>82</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>102</v>
+      </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="H15" s="5"/>
@@ -1130,9 +1451,11 @@
     </row>
     <row r="16" spans="1:23">
       <c r="A16" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="5"/>
+        <v>59</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>103</v>
+      </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="H16" s="5"/>
@@ -1154,9 +1477,11 @@
     </row>
     <row r="17" spans="1:23">
       <c r="A17" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17" s="5"/>
+        <v>60</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>104</v>
+      </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="H17" s="5"/>
@@ -1177,10 +1502,12 @@
       <c r="W17" s="7"/>
     </row>
     <row r="18" spans="1:23">
-      <c r="A18" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" s="5"/>
+      <c r="A18" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>105</v>
+      </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="H18" s="5"/>
@@ -1202,9 +1529,11 @@
     </row>
     <row r="19" spans="1:23">
       <c r="A19" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="5"/>
+        <v>61</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>179</v>
+      </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="H19" s="5"/>
@@ -1224,11 +1553,13 @@
       <c r="V19" s="1"/>
       <c r="W19" s="7"/>
     </row>
-    <row r="20" spans="1:23">
+    <row r="20" spans="1:23" ht="30.6">
       <c r="A20" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>106</v>
+      </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="H20" s="5"/>
@@ -1250,9 +1581,11 @@
     </row>
     <row r="21" spans="1:23">
       <c r="A21" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B21" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>178</v>
+      </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="H21" s="5"/>
@@ -1269,14 +1602,16 @@
       <c r="S21" s="5"/>
       <c r="T21" s="5"/>
       <c r="U21" s="5"/>
-      <c r="V21" s="1"/>
+      <c r="V21" s="5"/>
       <c r="W21" s="7"/>
     </row>
     <row r="22" spans="1:23">
       <c r="A22" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>107</v>
+      </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="H22" s="5"/>
@@ -1293,14 +1628,16 @@
       <c r="S22" s="5"/>
       <c r="T22" s="5"/>
       <c r="U22" s="5"/>
-      <c r="V22" s="1"/>
+      <c r="V22" s="5"/>
       <c r="W22" s="7"/>
     </row>
     <row r="23" spans="1:23">
       <c r="A23" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>108</v>
+      </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="H23" s="5"/>
@@ -1317,14 +1654,16 @@
       <c r="S23" s="5"/>
       <c r="T23" s="5"/>
       <c r="U23" s="5"/>
-      <c r="V23" s="5"/>
+      <c r="V23" s="1"/>
       <c r="W23" s="7"/>
     </row>
-    <row r="24" spans="1:23">
+    <row r="24" spans="1:23" ht="30.6">
       <c r="A24" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="5"/>
+        <v>84</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>109</v>
+      </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="H24" s="5"/>
@@ -1341,14 +1680,16 @@
       <c r="S24" s="5"/>
       <c r="T24" s="5"/>
       <c r="U24" s="5"/>
-      <c r="V24" s="5"/>
+      <c r="V24" s="1"/>
       <c r="W24" s="7"/>
     </row>
     <row r="25" spans="1:23">
       <c r="A25" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>110</v>
+      </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="H25" s="5"/>
@@ -1370,9 +1711,11 @@
     </row>
     <row r="26" spans="1:23">
       <c r="A26" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="B26" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>177</v>
+      </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="H26" s="5"/>
@@ -1394,9 +1737,11 @@
     </row>
     <row r="27" spans="1:23">
       <c r="A27" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>111</v>
+      </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="H27" s="5"/>
@@ -1418,9 +1763,11 @@
     </row>
     <row r="28" spans="1:23">
       <c r="A28" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="5"/>
+        <v>45</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>112</v>
+      </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="H28" s="5"/>
@@ -1440,11 +1787,13 @@
       <c r="V28" s="1"/>
       <c r="W28" s="7"/>
     </row>
-    <row r="29" spans="1:23">
-      <c r="A29" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" s="5"/>
+    <row r="29" spans="1:23" ht="30.6">
+      <c r="A29" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>113</v>
+      </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="H29" s="5"/>
@@ -1464,11 +1813,13 @@
       <c r="V29" s="1"/>
       <c r="W29" s="7"/>
     </row>
-    <row r="30" spans="1:23">
+    <row r="30" spans="1:23" ht="30.6">
       <c r="A30" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B30" s="5"/>
+        <v>79</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>114</v>
+      </c>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="H30" s="5"/>
@@ -1488,11 +1839,13 @@
       <c r="V30" s="1"/>
       <c r="W30" s="7"/>
     </row>
-    <row r="31" spans="1:23">
-      <c r="A31" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B31" s="5"/>
+    <row r="31" spans="1:23" ht="30.6">
+      <c r="A31" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>115</v>
+      </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="H31" s="5"/>
@@ -1514,9 +1867,11 @@
     </row>
     <row r="32" spans="1:23">
       <c r="A32" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B32" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>116</v>
+      </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="H32" s="5"/>
@@ -1538,9 +1893,11 @@
     </row>
     <row r="33" spans="1:23">
       <c r="A33" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B33" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>117</v>
+      </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="H33" s="5"/>
@@ -1562,9 +1919,11 @@
     </row>
     <row r="34" spans="1:23">
       <c r="A34" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B34" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>118</v>
+      </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="H34" s="5"/>
@@ -1586,9 +1945,11 @@
     </row>
     <row r="35" spans="1:23">
       <c r="A35" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>119</v>
+      </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="H35" s="5"/>
@@ -1605,14 +1966,16 @@
       <c r="S35" s="5"/>
       <c r="T35" s="5"/>
       <c r="U35" s="5"/>
-      <c r="V35" s="1"/>
+      <c r="V35" s="5"/>
       <c r="W35" s="7"/>
     </row>
     <row r="36" spans="1:23">
       <c r="A36" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B36" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>120</v>
+      </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="H36" s="5"/>
@@ -1629,14 +1992,16 @@
       <c r="S36" s="5"/>
       <c r="T36" s="5"/>
       <c r="U36" s="5"/>
-      <c r="V36" s="1"/>
+      <c r="V36" s="5"/>
       <c r="W36" s="7"/>
     </row>
-    <row r="37" spans="1:23">
+    <row r="37" spans="1:23" ht="30.6">
       <c r="A37" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B37" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>121</v>
+      </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="H37" s="5"/>
@@ -1653,14 +2018,16 @@
       <c r="S37" s="5"/>
       <c r="T37" s="5"/>
       <c r="U37" s="5"/>
-      <c r="V37" s="5"/>
+      <c r="V37" s="1"/>
       <c r="W37" s="7"/>
     </row>
-    <row r="38" spans="1:23">
+    <row r="38" spans="1:23" ht="30.6">
       <c r="A38" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38" s="5"/>
+        <v>65</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>122</v>
+      </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="H38" s="5"/>
@@ -1680,11 +2047,13 @@
       <c r="V38" s="5"/>
       <c r="W38" s="7"/>
     </row>
-    <row r="39" spans="1:23">
+    <row r="39" spans="1:23" ht="30.6">
       <c r="A39" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B39" s="5"/>
+        <v>66</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>123</v>
+      </c>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="H39" s="5"/>
@@ -1701,14 +2070,16 @@
       <c r="S39" s="5"/>
       <c r="T39" s="5"/>
       <c r="U39" s="5"/>
-      <c r="V39" s="1"/>
+      <c r="V39" s="5"/>
       <c r="W39" s="7"/>
     </row>
-    <row r="40" spans="1:23">
+    <row r="40" spans="1:23" ht="30.6">
       <c r="A40" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B40" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>124</v>
+      </c>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="H40" s="5"/>
@@ -1728,11 +2099,13 @@
       <c r="V40" s="5"/>
       <c r="W40" s="7"/>
     </row>
-    <row r="41" spans="1:23">
+    <row r="41" spans="1:23" ht="45.6">
       <c r="A41" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B41" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>125</v>
+      </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="H41" s="5"/>
@@ -1754,9 +2127,11 @@
     </row>
     <row r="42" spans="1:23">
       <c r="A42" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B42" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>175</v>
+      </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="H42" s="5"/>
@@ -1778,9 +2153,11 @@
     </row>
     <row r="43" spans="1:23">
       <c r="A43" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B43" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>176</v>
+      </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="H43" s="5"/>
@@ -1802,9 +2179,11 @@
     </row>
     <row r="44" spans="1:23">
       <c r="A44" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B44" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>126</v>
+      </c>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="H44" s="5"/>
@@ -1821,14 +2200,16 @@
       <c r="S44" s="5"/>
       <c r="T44" s="5"/>
       <c r="U44" s="5"/>
-      <c r="V44" s="5"/>
+      <c r="V44" s="1"/>
       <c r="W44" s="7"/>
     </row>
     <row r="45" spans="1:23">
       <c r="A45" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B45" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>127</v>
+      </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="H45" s="5"/>
@@ -1845,14 +2226,16 @@
       <c r="S45" s="5"/>
       <c r="T45" s="5"/>
       <c r="U45" s="5"/>
-      <c r="V45" s="5"/>
+      <c r="V45" s="1"/>
       <c r="W45" s="7"/>
     </row>
     <row r="46" spans="1:23">
       <c r="A46" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B46" s="5"/>
+        <v>38</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>128</v>
+      </c>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="H46" s="5"/>
@@ -1874,9 +2257,11 @@
     </row>
     <row r="47" spans="1:23">
       <c r="A47" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B47" s="5"/>
+        <v>63</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>129</v>
+      </c>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
       <c r="H47" s="5"/>
@@ -1896,11 +2281,13 @@
       <c r="V47" s="1"/>
       <c r="W47" s="7"/>
     </row>
-    <row r="48" spans="1:23">
-      <c r="A48" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B48" s="5"/>
+    <row r="48" spans="1:23" ht="30.6">
+      <c r="A48" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>130</v>
+      </c>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
       <c r="H48" s="5"/>
@@ -1922,9 +2309,11 @@
     </row>
     <row r="49" spans="1:23">
       <c r="A49" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B49" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>131</v>
+      </c>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
       <c r="H49" s="5"/>
@@ -1944,11 +2333,13 @@
       <c r="V49" s="1"/>
       <c r="W49" s="7"/>
     </row>
-    <row r="50" spans="1:23">
-      <c r="A50" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B50" s="5"/>
+    <row r="50" spans="1:23" ht="45.6">
+      <c r="A50" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>132</v>
+      </c>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="H50" s="5"/>
@@ -1968,11 +2359,13 @@
       <c r="V50" s="1"/>
       <c r="W50" s="7"/>
     </row>
-    <row r="51" spans="1:23">
+    <row r="51" spans="1:23" ht="45.6">
       <c r="A51" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B51" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>184</v>
+      </c>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
       <c r="H51" s="5"/>
@@ -1992,11 +2385,13 @@
       <c r="V51" s="1"/>
       <c r="W51" s="7"/>
     </row>
-    <row r="52" spans="1:23">
+    <row r="52" spans="1:23" ht="45.6">
       <c r="A52" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B52" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>133</v>
+      </c>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
       <c r="H52" s="5"/>
@@ -2016,11 +2411,13 @@
       <c r="V52" s="1"/>
       <c r="W52" s="7"/>
     </row>
-    <row r="53" spans="1:23">
+    <row r="53" spans="1:23" ht="30.6">
       <c r="A53" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B53" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>134</v>
+      </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
       <c r="H53" s="5"/>
@@ -2040,11 +2437,13 @@
       <c r="V53" s="1"/>
       <c r="W53" s="7"/>
     </row>
-    <row r="54" spans="1:23">
+    <row r="54" spans="1:23" ht="30.6">
       <c r="A54" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B54" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>135</v>
+      </c>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
       <c r="H54" s="5"/>
@@ -2064,11 +2463,13 @@
       <c r="V54" s="1"/>
       <c r="W54" s="7"/>
     </row>
-    <row r="55" spans="1:23">
-      <c r="A55" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B55" s="5"/>
+    <row r="55" spans="1:23" ht="30.6">
+      <c r="A55" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>136</v>
+      </c>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
       <c r="H55" s="5"/>
@@ -2085,14 +2486,16 @@
       <c r="S55" s="5"/>
       <c r="T55" s="5"/>
       <c r="U55" s="5"/>
-      <c r="V55" s="1"/>
+      <c r="V55" s="5"/>
       <c r="W55" s="7"/>
     </row>
-    <row r="56" spans="1:23">
-      <c r="A56" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B56" s="5"/>
+    <row r="56" spans="1:23" ht="30.6">
+      <c r="A56" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>137</v>
+      </c>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
       <c r="H56" s="5"/>
@@ -2109,14 +2512,16 @@
       <c r="S56" s="5"/>
       <c r="T56" s="5"/>
       <c r="U56" s="5"/>
-      <c r="V56" s="1"/>
+      <c r="V56" s="5"/>
       <c r="W56" s="7"/>
     </row>
     <row r="57" spans="1:23">
-      <c r="A57" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B57" s="5"/>
+      <c r="A57" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>138</v>
+      </c>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
       <c r="H57" s="5"/>
@@ -2137,10 +2542,12 @@
       <c r="W57" s="7"/>
     </row>
     <row r="58" spans="1:23">
-      <c r="A58" s="10" t="s">
+      <c r="A58" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B58" s="5"/>
+      <c r="B58" s="14" t="s">
+        <v>139</v>
+      </c>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
       <c r="H58" s="5"/>
@@ -2160,11 +2567,13 @@
       <c r="V58" s="5"/>
       <c r="W58" s="7"/>
     </row>
-    <row r="59" spans="1:23">
+    <row r="59" spans="1:23" ht="30.6">
       <c r="A59" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B59" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>140</v>
+      </c>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
       <c r="H59" s="5"/>
@@ -2184,11 +2593,13 @@
       <c r="V59" s="5"/>
       <c r="W59" s="7"/>
     </row>
-    <row r="60" spans="1:23">
+    <row r="60" spans="1:23" ht="45.6">
       <c r="A60" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B60" s="5"/>
+        <v>92</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>185</v>
+      </c>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
       <c r="H60" s="5"/>
@@ -2208,11 +2619,13 @@
       <c r="V60" s="5"/>
       <c r="W60" s="7"/>
     </row>
-    <row r="61" spans="1:23">
+    <row r="61" spans="1:23" ht="30.6">
       <c r="A61" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B61" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>141</v>
+      </c>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
       <c r="H61" s="5"/>
@@ -2232,11 +2645,13 @@
       <c r="V61" s="5"/>
       <c r="W61" s="7"/>
     </row>
-    <row r="62" spans="1:23">
+    <row r="62" spans="1:23" ht="30.6">
       <c r="A62" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B62" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>142</v>
+      </c>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
       <c r="H62" s="5"/>
@@ -2256,11 +2671,13 @@
       <c r="V62" s="5"/>
       <c r="W62" s="7"/>
     </row>
-    <row r="63" spans="1:23">
+    <row r="63" spans="1:23" ht="30.6">
       <c r="A63" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B63" s="5"/>
+        <v>54</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>143</v>
+      </c>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
       <c r="H63" s="5"/>
@@ -2282,9 +2699,11 @@
     </row>
     <row r="64" spans="1:23">
       <c r="A64" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B64" s="5"/>
+        <v>57</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>144</v>
+      </c>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
       <c r="H64" s="5"/>
@@ -2306,9 +2725,11 @@
     </row>
     <row r="65" spans="1:23">
       <c r="A65" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B65" s="5"/>
+        <v>58</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>145</v>
+      </c>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
       <c r="H65" s="5"/>
@@ -2328,11 +2749,13 @@
       <c r="V65" s="5"/>
       <c r="W65" s="7"/>
     </row>
-    <row r="66" spans="1:23">
+    <row r="66" spans="1:23" ht="30.6">
       <c r="A66" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B66" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>146</v>
+      </c>
       <c r="D66" s="5"/>
       <c r="E66" s="5"/>
       <c r="H66" s="5"/>
@@ -2352,11 +2775,13 @@
       <c r="V66" s="5"/>
       <c r="W66" s="7"/>
     </row>
-    <row r="67" spans="1:23">
+    <row r="67" spans="1:23" ht="30.6">
       <c r="A67" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B67" s="5"/>
+        <v>11</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>147</v>
+      </c>
       <c r="D67" s="5"/>
       <c r="E67" s="5"/>
       <c r="H67" s="5"/>
@@ -2376,11 +2801,13 @@
       <c r="V67" s="5"/>
       <c r="W67" s="7"/>
     </row>
-    <row r="68" spans="1:23">
+    <row r="68" spans="1:23" ht="45.6">
       <c r="A68" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B68" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>148</v>
+      </c>
       <c r="D68" s="5"/>
       <c r="E68" s="5"/>
       <c r="H68" s="5"/>
@@ -2400,11 +2827,13 @@
       <c r="V68" s="5"/>
       <c r="W68" s="7"/>
     </row>
-    <row r="69" spans="1:23">
+    <row r="69" spans="1:23" ht="45.6">
       <c r="A69" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B69" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>149</v>
+      </c>
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
       <c r="H69" s="5"/>
@@ -2426,9 +2855,11 @@
     </row>
     <row r="70" spans="1:23">
       <c r="A70" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B70" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="B70" s="14" t="s">
+        <v>150</v>
+      </c>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
       <c r="H70" s="5"/>
@@ -2445,14 +2876,16 @@
       <c r="S70" s="5"/>
       <c r="T70" s="5"/>
       <c r="U70" s="5"/>
-      <c r="V70" s="5"/>
+      <c r="V70" s="1"/>
       <c r="W70" s="7"/>
     </row>
-    <row r="71" spans="1:23">
+    <row r="71" spans="1:23" ht="45.6">
       <c r="A71" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B71" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="B71" s="14" t="s">
+        <v>151</v>
+      </c>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
       <c r="H71" s="5"/>
@@ -2469,14 +2902,16 @@
       <c r="S71" s="5"/>
       <c r="T71" s="5"/>
       <c r="U71" s="5"/>
-      <c r="V71" s="5"/>
+      <c r="V71" s="1"/>
       <c r="W71" s="7"/>
     </row>
-    <row r="72" spans="1:23">
+    <row r="72" spans="1:23" ht="30.6">
       <c r="A72" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B72" s="5"/>
+        <v>6</v>
+      </c>
+      <c r="B72" s="14" t="s">
+        <v>152</v>
+      </c>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
       <c r="H72" s="5"/>
@@ -2496,11 +2931,13 @@
       <c r="V72" s="1"/>
       <c r="W72" s="7"/>
     </row>
-    <row r="73" spans="1:23">
+    <row r="73" spans="1:23" ht="45.6">
       <c r="A73" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B73" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>153</v>
+      </c>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
       <c r="H73" s="5"/>
@@ -2517,14 +2954,16 @@
       <c r="S73" s="5"/>
       <c r="T73" s="5"/>
       <c r="U73" s="5"/>
-      <c r="V73" s="1"/>
+      <c r="V73" s="5"/>
       <c r="W73" s="7"/>
     </row>
-    <row r="74" spans="1:23">
-      <c r="A74" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B74" s="5"/>
+    <row r="74" spans="1:23" ht="30.6">
+      <c r="A74" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B74" s="14" t="s">
+        <v>154</v>
+      </c>
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
       <c r="H74" s="5"/>
@@ -2541,14 +2980,16 @@
       <c r="S74" s="5"/>
       <c r="T74" s="5"/>
       <c r="U74" s="5"/>
-      <c r="V74" s="1"/>
+      <c r="V74" s="5"/>
       <c r="W74" s="7"/>
     </row>
-    <row r="75" spans="1:23">
-      <c r="A75" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B75" s="5"/>
+    <row r="75" spans="1:23" ht="45.6">
+      <c r="A75" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B75" s="14" t="s">
+        <v>155</v>
+      </c>
       <c r="D75" s="5"/>
       <c r="E75" s="5"/>
       <c r="H75" s="5"/>
@@ -2565,14 +3006,16 @@
       <c r="S75" s="5"/>
       <c r="T75" s="5"/>
       <c r="U75" s="5"/>
-      <c r="V75" s="5"/>
+      <c r="V75" s="1"/>
       <c r="W75" s="7"/>
     </row>
     <row r="76" spans="1:23">
-      <c r="A76" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B76" s="5"/>
+      <c r="A76" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B76" s="14" t="s">
+        <v>156</v>
+      </c>
       <c r="D76" s="5"/>
       <c r="E76" s="5"/>
       <c r="H76" s="5"/>
@@ -2589,14 +3032,16 @@
       <c r="S76" s="5"/>
       <c r="T76" s="5"/>
       <c r="U76" s="5"/>
-      <c r="V76" s="5"/>
+      <c r="V76" s="1"/>
       <c r="W76" s="7"/>
     </row>
     <row r="77" spans="1:23">
-      <c r="A77" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B77" s="5"/>
+      <c r="A77" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>157</v>
+      </c>
       <c r="D77" s="5"/>
       <c r="E77" s="5"/>
       <c r="H77" s="5"/>
@@ -2617,10 +3062,12 @@
       <c r="W77" s="7"/>
     </row>
     <row r="78" spans="1:23">
-      <c r="A78" s="11" t="s">
+      <c r="A78" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="B78" s="5"/>
+      <c r="B78" s="14" t="s">
+        <v>158</v>
+      </c>
       <c r="D78" s="5"/>
       <c r="E78" s="5"/>
       <c r="H78" s="5"/>
@@ -2642,9 +3089,11 @@
     </row>
     <row r="79" spans="1:23">
       <c r="A79" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="B79" s="5"/>
+        <v>86</v>
+      </c>
+      <c r="B79" s="14" t="s">
+        <v>159</v>
+      </c>
       <c r="D79" s="5"/>
       <c r="E79" s="5"/>
       <c r="H79" s="5"/>
@@ -2661,14 +3110,16 @@
       <c r="S79" s="5"/>
       <c r="T79" s="5"/>
       <c r="U79" s="5"/>
-      <c r="V79" s="1"/>
+      <c r="V79" s="5"/>
       <c r="W79" s="7"/>
     </row>
     <row r="80" spans="1:23">
       <c r="A80" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="B80" s="5"/>
+        <v>90</v>
+      </c>
+      <c r="B80" s="14" t="s">
+        <v>160</v>
+      </c>
       <c r="D80" s="5"/>
       <c r="E80" s="5"/>
       <c r="H80" s="5"/>
@@ -2685,14 +3136,16 @@
       <c r="S80" s="5"/>
       <c r="T80" s="5"/>
       <c r="U80" s="5"/>
-      <c r="V80" s="1"/>
+      <c r="V80" s="5"/>
       <c r="W80" s="7"/>
     </row>
     <row r="81" spans="1:23">
       <c r="A81" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B81" s="5"/>
+        <v>91</v>
+      </c>
+      <c r="B81" s="14" t="s">
+        <v>161</v>
+      </c>
       <c r="D81" s="5"/>
       <c r="E81" s="5"/>
       <c r="H81" s="5"/>
@@ -2712,11 +3165,13 @@
       <c r="V81" s="5"/>
       <c r="W81" s="7"/>
     </row>
-    <row r="82" spans="1:23">
-      <c r="A82" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="B82" s="5"/>
+    <row r="82" spans="1:23" ht="31.2">
+      <c r="A82" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B82" s="15" t="s">
+        <v>162</v>
+      </c>
       <c r="D82" s="5"/>
       <c r="E82" s="5"/>
       <c r="H82" s="5"/>
@@ -2737,10 +3192,12 @@
       <c r="W82" s="7"/>
     </row>
     <row r="83" spans="1:23">
-      <c r="A83" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="B83" s="5"/>
+      <c r="A83" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B83" s="15" t="s">
+        <v>163</v>
+      </c>
       <c r="D83" s="5"/>
       <c r="E83" s="5"/>
       <c r="H83" s="5"/>
@@ -2762,9 +3219,11 @@
     </row>
     <row r="84" spans="1:23">
       <c r="A84" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B84" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="B84" s="15" t="s">
+        <v>164</v>
+      </c>
       <c r="D84" s="5"/>
       <c r="E84" s="5"/>
       <c r="H84" s="5"/>
@@ -2786,9 +3245,11 @@
     </row>
     <row r="85" spans="1:23">
       <c r="A85" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B85" s="5"/>
+        <v>70</v>
+      </c>
+      <c r="B85" s="15" t="s">
+        <v>165</v>
+      </c>
       <c r="D85" s="5"/>
       <c r="E85" s="5"/>
       <c r="H85" s="5"/>
@@ -2808,11 +3269,13 @@
       <c r="V85" s="5"/>
       <c r="W85" s="7"/>
     </row>
-    <row r="86" spans="1:23">
+    <row r="86" spans="1:23" ht="46.8">
       <c r="A86" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B86" s="5"/>
+        <v>71</v>
+      </c>
+      <c r="B86" s="15" t="s">
+        <v>166</v>
+      </c>
       <c r="D86" s="5"/>
       <c r="E86" s="5"/>
       <c r="H86" s="5"/>
@@ -2836,7 +3299,9 @@
       <c r="A87" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="B87" s="5"/>
+      <c r="B87" s="15" t="s">
+        <v>167</v>
+      </c>
       <c r="D87" s="5"/>
       <c r="E87" s="5"/>
       <c r="H87" s="5"/>
@@ -2860,7 +3325,9 @@
       <c r="A88" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B88" s="5"/>
+      <c r="B88" s="15" t="s">
+        <v>168</v>
+      </c>
       <c r="D88" s="5"/>
       <c r="E88" s="5"/>
       <c r="H88" s="5"/>
@@ -2884,7 +3351,9 @@
       <c r="A89" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="B89" s="5"/>
+      <c r="B89" s="15" t="s">
+        <v>169</v>
+      </c>
       <c r="D89" s="5"/>
       <c r="E89" s="5"/>
       <c r="H89" s="5"/>
@@ -2904,11 +3373,14 @@
       <c r="V89" s="5"/>
       <c r="W89" s="7"/>
     </row>
-    <row r="90" spans="1:23">
+    <row r="90" spans="1:23" ht="31.2">
       <c r="A90" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="B90" s="5"/>
+      <c r="B90" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="C90" s="5"/>
       <c r="D90" s="5"/>
       <c r="E90" s="5"/>
       <c r="H90" s="5"/>
@@ -2928,11 +3400,14 @@
       <c r="V90" s="5"/>
       <c r="W90" s="7"/>
     </row>
-    <row r="91" spans="1:23">
+    <row r="91" spans="1:23" ht="31.2">
       <c r="A91" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B91" s="5"/>
+      <c r="B91" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="C91" s="5"/>
       <c r="D91" s="5"/>
       <c r="E91" s="5"/>
       <c r="H91" s="5"/>
@@ -2956,7 +3431,9 @@
       <c r="A92" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B92" s="5"/>
+      <c r="B92" s="15" t="s">
+        <v>172</v>
+      </c>
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
       <c r="E92" s="5"/>
@@ -2977,11 +3454,13 @@
       <c r="V92" s="5"/>
       <c r="W92" s="7"/>
     </row>
-    <row r="93" spans="1:23">
+    <row r="93" spans="1:23" ht="31.2">
       <c r="A93" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B93" s="5"/>
+      <c r="B93" s="15" t="s">
+        <v>173</v>
+      </c>
       <c r="C93" s="5"/>
       <c r="D93" s="5"/>
       <c r="E93" s="5"/>
@@ -3003,9 +3482,6 @@
       <c r="W93" s="7"/>
     </row>
     <row r="94" spans="1:23">
-      <c r="A94" s="12" t="s">
-        <v>79</v>
-      </c>
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
       <c r="D94" s="5"/>
@@ -3028,9 +3504,6 @@
       <c r="W94" s="7"/>
     </row>
     <row r="95" spans="1:23">
-      <c r="A95" s="12" t="s">
-        <v>80</v>
-      </c>
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
       <c r="D95" s="5"/>
@@ -3049,10 +3522,11 @@
       <c r="S95" s="5"/>
       <c r="T95" s="5"/>
       <c r="U95" s="5"/>
-      <c r="V95" s="5"/>
+      <c r="V95" s="1"/>
       <c r="W95" s="7"/>
     </row>
     <row r="96" spans="1:23">
+      <c r="A96" s="3"/>
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
       <c r="D96" s="5"/>
@@ -3071,10 +3545,11 @@
       <c r="S96" s="5"/>
       <c r="T96" s="5"/>
       <c r="U96" s="5"/>
-      <c r="V96" s="5"/>
+      <c r="V96" s="1"/>
       <c r="W96" s="7"/>
     </row>
     <row r="97" spans="1:23">
+      <c r="A97" s="3"/>
       <c r="B97" s="5"/>
       <c r="C97" s="5"/>
       <c r="D97" s="5"/>
@@ -3093,7 +3568,7 @@
       <c r="S97" s="5"/>
       <c r="T97" s="5"/>
       <c r="U97" s="5"/>
-      <c r="V97" s="1"/>
+      <c r="V97" s="5"/>
       <c r="W97" s="7"/>
     </row>
     <row r="98" spans="1:23">
@@ -3116,7 +3591,7 @@
       <c r="S98" s="5"/>
       <c r="T98" s="5"/>
       <c r="U98" s="5"/>
-      <c r="V98" s="1"/>
+      <c r="V98" s="5"/>
       <c r="W98" s="7"/>
     </row>
     <row r="99" spans="1:23">
@@ -3231,7 +3706,7 @@
       <c r="S103" s="5"/>
       <c r="T103" s="5"/>
       <c r="U103" s="5"/>
-      <c r="V103" s="5"/>
+      <c r="V103" s="1"/>
       <c r="W103" s="7"/>
     </row>
     <row r="104" spans="1:23">
@@ -3254,7 +3729,7 @@
       <c r="S104" s="5"/>
       <c r="T104" s="5"/>
       <c r="U104" s="5"/>
-      <c r="V104" s="5"/>
+      <c r="V104" s="1"/>
       <c r="W104" s="7"/>
     </row>
     <row r="105" spans="1:23">
@@ -3277,7 +3752,7 @@
       <c r="S105" s="5"/>
       <c r="T105" s="5"/>
       <c r="U105" s="5"/>
-      <c r="V105" s="1"/>
+      <c r="V105" s="5"/>
       <c r="W105" s="7"/>
     </row>
     <row r="106" spans="1:23">
@@ -3300,7 +3775,7 @@
       <c r="S106" s="5"/>
       <c r="T106" s="5"/>
       <c r="U106" s="5"/>
-      <c r="V106" s="1"/>
+      <c r="V106" s="5"/>
       <c r="W106" s="7"/>
     </row>
     <row r="107" spans="1:23">
@@ -3350,7 +3825,6 @@
       <c r="W108" s="7"/>
     </row>
     <row r="109" spans="1:23">
-      <c r="A109" s="3"/>
       <c r="B109" s="5"/>
       <c r="C109" s="5"/>
       <c r="D109" s="5"/>
@@ -3373,7 +3847,6 @@
       <c r="W109" s="7"/>
     </row>
     <row r="110" spans="1:23">
-      <c r="A110" s="3"/>
       <c r="B110" s="5"/>
       <c r="C110" s="5"/>
       <c r="D110" s="5"/>
@@ -3458,7 +3931,7 @@
       <c r="S113" s="5"/>
       <c r="T113" s="5"/>
       <c r="U113" s="5"/>
-      <c r="V113" s="5"/>
+      <c r="V113" s="1"/>
       <c r="W113" s="7"/>
     </row>
     <row r="114" spans="1:23">
@@ -3480,7 +3953,7 @@
       <c r="S114" s="5"/>
       <c r="T114" s="5"/>
       <c r="U114" s="5"/>
-      <c r="V114" s="5"/>
+      <c r="V114" s="1"/>
       <c r="W114" s="7"/>
     </row>
     <row r="115" spans="1:23">
@@ -3638,6 +4111,7 @@
       <c r="W121" s="7"/>
     </row>
     <row r="122" spans="1:23">
+      <c r="A122" s="3"/>
       <c r="B122" s="5"/>
       <c r="C122" s="5"/>
       <c r="D122" s="5"/>
@@ -3678,11 +4152,10 @@
       <c r="S123" s="5"/>
       <c r="T123" s="5"/>
       <c r="U123" s="5"/>
-      <c r="V123" s="1"/>
+      <c r="V123" s="5"/>
       <c r="W123" s="7"/>
     </row>
     <row r="124" spans="1:23">
-      <c r="A124" s="3"/>
       <c r="B124" s="5"/>
       <c r="C124" s="5"/>
       <c r="D124" s="5"/>
@@ -3701,7 +4174,7 @@
       <c r="S124" s="5"/>
       <c r="T124" s="5"/>
       <c r="U124" s="5"/>
-      <c r="V124" s="1"/>
+      <c r="V124" s="5"/>
       <c r="W124" s="7"/>
     </row>
     <row r="125" spans="1:23">
@@ -3723,7 +4196,7 @@
       <c r="S125" s="5"/>
       <c r="T125" s="5"/>
       <c r="U125" s="5"/>
-      <c r="V125" s="5"/>
+      <c r="V125" s="1"/>
       <c r="W125" s="7"/>
     </row>
     <row r="126" spans="1:23">
@@ -3767,7 +4240,7 @@
       <c r="S127" s="5"/>
       <c r="T127" s="5"/>
       <c r="U127" s="5"/>
-      <c r="V127" s="1"/>
+      <c r="V127" s="5"/>
       <c r="W127" s="7"/>
     </row>
     <row r="128" spans="1:23">
@@ -3789,10 +4262,11 @@
       <c r="S128" s="5"/>
       <c r="T128" s="5"/>
       <c r="U128" s="5"/>
-      <c r="V128" s="5"/>
+      <c r="V128" s="1"/>
       <c r="W128" s="7"/>
     </row>
     <row r="129" spans="1:23">
+      <c r="A129" s="3"/>
       <c r="B129" s="5"/>
       <c r="C129" s="5"/>
       <c r="D129" s="5"/>
@@ -3811,7 +4285,7 @@
       <c r="S129" s="5"/>
       <c r="T129" s="5"/>
       <c r="U129" s="5"/>
-      <c r="V129" s="5"/>
+      <c r="V129" s="1"/>
       <c r="W129" s="7"/>
     </row>
     <row r="130" spans="1:23">
@@ -3882,7 +4356,6 @@
       <c r="W132" s="7"/>
     </row>
     <row r="133" spans="1:23">
-      <c r="A133" s="3"/>
       <c r="B133" s="5"/>
       <c r="C133" s="5"/>
       <c r="D133" s="5"/>
@@ -3989,7 +4462,7 @@
       <c r="S137" s="5"/>
       <c r="T137" s="5"/>
       <c r="U137" s="5"/>
-      <c r="V137" s="1"/>
+      <c r="V137" s="5"/>
       <c r="W137" s="7"/>
     </row>
     <row r="138" spans="1:23">
@@ -4011,7 +4484,7 @@
       <c r="S138" s="5"/>
       <c r="T138" s="5"/>
       <c r="U138" s="5"/>
-      <c r="V138" s="1"/>
+      <c r="V138" s="5"/>
       <c r="W138" s="7"/>
     </row>
     <row r="139" spans="1:23">
@@ -4033,7 +4506,7 @@
       <c r="S139" s="5"/>
       <c r="T139" s="5"/>
       <c r="U139" s="5"/>
-      <c r="V139" s="5"/>
+      <c r="V139" s="1"/>
       <c r="W139" s="7"/>
     </row>
     <row r="140" spans="1:23">
@@ -4077,7 +4550,7 @@
       <c r="S141" s="5"/>
       <c r="T141" s="5"/>
       <c r="U141" s="5"/>
-      <c r="V141" s="1"/>
+      <c r="V141" s="5"/>
       <c r="W141" s="7"/>
     </row>
     <row r="142" spans="1:23">
@@ -4121,7 +4594,7 @@
       <c r="S143" s="5"/>
       <c r="T143" s="5"/>
       <c r="U143" s="5"/>
-      <c r="V143" s="5"/>
+      <c r="V143" s="1"/>
       <c r="W143" s="7"/>
     </row>
     <row r="144" spans="1:23">
@@ -4143,7 +4616,7 @@
       <c r="S144" s="5"/>
       <c r="T144" s="5"/>
       <c r="U144" s="5"/>
-      <c r="V144" s="5"/>
+      <c r="V144" s="1"/>
       <c r="W144" s="7"/>
     </row>
     <row r="145" spans="2:23">
@@ -4165,7 +4638,7 @@
       <c r="S145" s="5"/>
       <c r="T145" s="5"/>
       <c r="U145" s="5"/>
-      <c r="V145" s="1"/>
+      <c r="V145" s="5"/>
       <c r="W145" s="7"/>
     </row>
     <row r="146" spans="2:23">
@@ -4187,7 +4660,7 @@
       <c r="S146" s="5"/>
       <c r="T146" s="5"/>
       <c r="U146" s="5"/>
-      <c r="V146" s="1"/>
+      <c r="V146" s="5"/>
       <c r="W146" s="7"/>
     </row>
     <row r="147" spans="2:23">
@@ -4517,7 +4990,7 @@
       <c r="S161" s="5"/>
       <c r="T161" s="5"/>
       <c r="U161" s="5"/>
-      <c r="V161" s="5"/>
+      <c r="V161" s="1"/>
       <c r="W161" s="7"/>
     </row>
     <row r="162" spans="2:23">
@@ -4539,7 +5012,7 @@
       <c r="S162" s="5"/>
       <c r="T162" s="5"/>
       <c r="U162" s="5"/>
-      <c r="V162" s="5"/>
+      <c r="V162" s="1"/>
       <c r="W162" s="7"/>
     </row>
     <row r="163" spans="2:23">
@@ -4561,7 +5034,7 @@
       <c r="S163" s="5"/>
       <c r="T163" s="5"/>
       <c r="U163" s="5"/>
-      <c r="V163" s="1"/>
+      <c r="V163" s="5"/>
       <c r="W163" s="7"/>
     </row>
     <row r="164" spans="2:23">
@@ -4583,7 +5056,7 @@
       <c r="S164" s="5"/>
       <c r="T164" s="5"/>
       <c r="U164" s="5"/>
-      <c r="V164" s="1"/>
+      <c r="V164" s="5"/>
       <c r="W164" s="7"/>
     </row>
     <row r="165" spans="2:23">
@@ -4605,7 +5078,7 @@
       <c r="S165" s="5"/>
       <c r="T165" s="5"/>
       <c r="U165" s="5"/>
-      <c r="V165" s="5"/>
+      <c r="V165" s="1"/>
       <c r="W165" s="7"/>
     </row>
     <row r="166" spans="2:23">
@@ -4627,7 +5100,7 @@
       <c r="S166" s="5"/>
       <c r="T166" s="5"/>
       <c r="U166" s="5"/>
-      <c r="V166" s="5"/>
+      <c r="V166" s="1"/>
       <c r="W166" s="7"/>
     </row>
     <row r="167" spans="2:23">
@@ -4649,7 +5122,7 @@
       <c r="S167" s="5"/>
       <c r="T167" s="5"/>
       <c r="U167" s="5"/>
-      <c r="V167" s="1"/>
+      <c r="V167" s="5"/>
       <c r="W167" s="7"/>
     </row>
     <row r="168" spans="2:23">
@@ -4671,7 +5144,7 @@
       <c r="S168" s="5"/>
       <c r="T168" s="5"/>
       <c r="U168" s="5"/>
-      <c r="V168" s="1"/>
+      <c r="V168" s="5"/>
       <c r="W168" s="7"/>
     </row>
     <row r="169" spans="2:23">
@@ -5001,7 +5474,7 @@
       <c r="S183" s="5"/>
       <c r="T183" s="5"/>
       <c r="U183" s="5"/>
-      <c r="V183" s="5"/>
+      <c r="V183" s="1"/>
       <c r="W183" s="7"/>
     </row>
     <row r="184" spans="2:23">
@@ -5023,7 +5496,7 @@
       <c r="S184" s="5"/>
       <c r="T184" s="5"/>
       <c r="U184" s="5"/>
-      <c r="V184" s="5"/>
+      <c r="V184" s="1"/>
       <c r="W184" s="7"/>
     </row>
     <row r="185" spans="2:23">
@@ -5089,7 +5562,7 @@
       <c r="S187" s="5"/>
       <c r="T187" s="5"/>
       <c r="U187" s="5"/>
-      <c r="V187" s="1"/>
+      <c r="V187" s="5"/>
       <c r="W187" s="7"/>
     </row>
     <row r="188" spans="2:23">
@@ -5111,7 +5584,7 @@
       <c r="S188" s="5"/>
       <c r="T188" s="5"/>
       <c r="U188" s="5"/>
-      <c r="V188" s="1"/>
+      <c r="V188" s="5"/>
       <c r="W188" s="7"/>
     </row>
     <row r="189" spans="2:23">
@@ -5177,7 +5650,7 @@
       <c r="S191" s="5"/>
       <c r="T191" s="5"/>
       <c r="U191" s="5"/>
-      <c r="V191" s="5"/>
+      <c r="V191" s="1"/>
       <c r="W191" s="7"/>
     </row>
     <row r="192" spans="2:23">
@@ -5199,7 +5672,7 @@
       <c r="S192" s="5"/>
       <c r="T192" s="5"/>
       <c r="U192" s="5"/>
-      <c r="V192" s="5"/>
+      <c r="V192" s="1"/>
       <c r="W192" s="7"/>
     </row>
     <row r="193" spans="2:23">
@@ -5221,7 +5694,7 @@
       <c r="S193" s="5"/>
       <c r="T193" s="5"/>
       <c r="U193" s="5"/>
-      <c r="V193" s="1"/>
+      <c r="V193" s="5"/>
       <c r="W193" s="7"/>
     </row>
     <row r="194" spans="2:23">
@@ -5243,7 +5716,7 @@
       <c r="S194" s="5"/>
       <c r="T194" s="5"/>
       <c r="U194" s="5"/>
-      <c r="V194" s="1"/>
+      <c r="V194" s="5"/>
       <c r="W194" s="7"/>
     </row>
     <row r="195" spans="2:23">
@@ -5441,7 +5914,7 @@
       <c r="S203" s="5"/>
       <c r="T203" s="5"/>
       <c r="U203" s="5"/>
-      <c r="V203" s="5"/>
+      <c r="V203" s="1"/>
       <c r="W203" s="7"/>
     </row>
     <row r="204" spans="2:23">
@@ -5463,7 +5936,7 @@
       <c r="S204" s="5"/>
       <c r="T204" s="5"/>
       <c r="U204" s="5"/>
-      <c r="V204" s="5"/>
+      <c r="V204" s="1"/>
       <c r="W204" s="7"/>
     </row>
     <row r="205" spans="2:23">
@@ -5485,7 +5958,7 @@
       <c r="S205" s="5"/>
       <c r="T205" s="5"/>
       <c r="U205" s="5"/>
-      <c r="V205" s="1"/>
+      <c r="V205" s="5"/>
       <c r="W205" s="7"/>
     </row>
     <row r="206" spans="2:23">
@@ -5507,7 +5980,7 @@
       <c r="S206" s="5"/>
       <c r="T206" s="5"/>
       <c r="U206" s="5"/>
-      <c r="V206" s="1"/>
+      <c r="V206" s="5"/>
       <c r="W206" s="7"/>
     </row>
     <row r="207" spans="2:23">
@@ -5555,6 +6028,7 @@
       <c r="W208" s="7"/>
     </row>
     <row r="209" spans="1:23">
+      <c r="A209" s="3"/>
       <c r="B209" s="5"/>
       <c r="C209" s="5"/>
       <c r="D209" s="5"/>
@@ -5573,7 +6047,7 @@
       <c r="S209" s="5"/>
       <c r="T209" s="5"/>
       <c r="U209" s="5"/>
-      <c r="V209" s="5"/>
+      <c r="V209" s="1"/>
       <c r="W209" s="7"/>
     </row>
     <row r="210" spans="1:23">
@@ -5595,11 +6069,11 @@
       <c r="S210" s="5"/>
       <c r="T210" s="5"/>
       <c r="U210" s="5"/>
-      <c r="V210" s="5"/>
+      <c r="V210" s="1"/>
       <c r="W210" s="7"/>
     </row>
     <row r="211" spans="1:23">
-      <c r="A211" s="3"/>
+      <c r="A211" s="8"/>
       <c r="B211" s="5"/>
       <c r="C211" s="5"/>
       <c r="D211" s="5"/>
@@ -5618,10 +6092,11 @@
       <c r="S211" s="5"/>
       <c r="T211" s="5"/>
       <c r="U211" s="5"/>
-      <c r="V211" s="1"/>
+      <c r="V211" s="5"/>
       <c r="W211" s="7"/>
     </row>
     <row r="212" spans="1:23">
+      <c r="A212" s="3"/>
       <c r="B212" s="5"/>
       <c r="C212" s="5"/>
       <c r="D212" s="5"/>
@@ -5640,11 +6115,11 @@
       <c r="S212" s="5"/>
       <c r="T212" s="5"/>
       <c r="U212" s="5"/>
-      <c r="V212" s="1"/>
+      <c r="V212" s="5"/>
       <c r="W212" s="7"/>
     </row>
     <row r="213" spans="1:23">
-      <c r="A213" s="8"/>
+      <c r="A213" s="3"/>
       <c r="B213" s="5"/>
       <c r="C213" s="5"/>
       <c r="D213" s="5"/>
@@ -5667,7 +6142,6 @@
       <c r="W213" s="7"/>
     </row>
     <row r="214" spans="1:23">
-      <c r="A214" s="3"/>
       <c r="B214" s="5"/>
       <c r="C214" s="5"/>
       <c r="D214" s="5"/>
@@ -5690,7 +6164,6 @@
       <c r="W214" s="7"/>
     </row>
     <row r="215" spans="1:23">
-      <c r="A215" s="3"/>
       <c r="B215" s="5"/>
       <c r="C215" s="5"/>
       <c r="D215" s="5"/>
@@ -6153,6 +6626,7 @@
       <c r="W235" s="7"/>
     </row>
     <row r="236" spans="1:23">
+      <c r="A236" s="8"/>
       <c r="B236" s="5"/>
       <c r="C236" s="5"/>
       <c r="D236" s="5"/>
@@ -6193,7 +6667,7 @@
       <c r="S237" s="5"/>
       <c r="T237" s="5"/>
       <c r="U237" s="5"/>
-      <c r="V237" s="5"/>
+      <c r="V237" s="1"/>
       <c r="W237" s="7"/>
     </row>
     <row r="238" spans="1:23">
@@ -6216,10 +6690,11 @@
       <c r="S238" s="5"/>
       <c r="T238" s="5"/>
       <c r="U238" s="5"/>
-      <c r="V238" s="5"/>
+      <c r="V238" s="1"/>
       <c r="W238" s="7"/>
     </row>
     <row r="239" spans="1:23">
+      <c r="A239" s="3"/>
       <c r="B239" s="5"/>
       <c r="C239" s="5"/>
       <c r="D239" s="5"/>
@@ -6238,11 +6713,10 @@
       <c r="S239" s="5"/>
       <c r="T239" s="5"/>
       <c r="U239" s="5"/>
-      <c r="V239" s="1"/>
+      <c r="V239" s="5"/>
       <c r="W239" s="7"/>
     </row>
     <row r="240" spans="1:23">
-      <c r="A240" s="8"/>
       <c r="B240" s="5"/>
       <c r="C240" s="5"/>
       <c r="D240" s="5"/>
@@ -6261,11 +6735,10 @@
       <c r="S240" s="5"/>
       <c r="T240" s="5"/>
       <c r="U240" s="5"/>
-      <c r="V240" s="1"/>
+      <c r="V240" s="5"/>
       <c r="W240" s="7"/>
     </row>
     <row r="241" spans="1:23">
-      <c r="A241" s="3"/>
       <c r="B241" s="5"/>
       <c r="C241" s="5"/>
       <c r="D241" s="5"/>
@@ -6284,7 +6757,7 @@
       <c r="S241" s="5"/>
       <c r="T241" s="5"/>
       <c r="U241" s="5"/>
-      <c r="V241" s="5"/>
+      <c r="V241" s="1"/>
       <c r="W241" s="7"/>
     </row>
     <row r="242" spans="1:23">
@@ -6310,6 +6783,7 @@
       <c r="W242" s="7"/>
     </row>
     <row r="243" spans="1:23">
+      <c r="A243" s="8"/>
       <c r="B243" s="5"/>
       <c r="C243" s="5"/>
       <c r="D243" s="5"/>
@@ -6328,7 +6802,7 @@
       <c r="S243" s="5"/>
       <c r="T243" s="5"/>
       <c r="U243" s="5"/>
-      <c r="V243" s="1"/>
+      <c r="V243" s="5"/>
       <c r="W243" s="7"/>
     </row>
     <row r="244" spans="1:23">
@@ -6350,7 +6824,7 @@
       <c r="S244" s="5"/>
       <c r="T244" s="5"/>
       <c r="U244" s="5"/>
-      <c r="V244" s="5"/>
+      <c r="V244" s="1"/>
       <c r="W244" s="7"/>
     </row>
     <row r="245" spans="1:23">
@@ -6373,7 +6847,7 @@
       <c r="S245" s="5"/>
       <c r="T245" s="5"/>
       <c r="U245" s="5"/>
-      <c r="V245" s="5"/>
+      <c r="V245" s="1"/>
       <c r="W245" s="7"/>
     </row>
     <row r="246" spans="1:23">
@@ -6399,7 +6873,6 @@
       <c r="W246" s="7"/>
     </row>
     <row r="247" spans="1:23">
-      <c r="A247" s="8"/>
       <c r="B247" s="5"/>
       <c r="C247" s="5"/>
       <c r="D247" s="5"/>
@@ -6440,7 +6913,7 @@
       <c r="S248" s="5"/>
       <c r="T248" s="5"/>
       <c r="U248" s="5"/>
-      <c r="V248" s="1"/>
+      <c r="V248" s="5"/>
       <c r="W248" s="7"/>
     </row>
     <row r="249" spans="1:23">
@@ -6462,7 +6935,7 @@
       <c r="S249" s="5"/>
       <c r="T249" s="5"/>
       <c r="U249" s="5"/>
-      <c r="V249" s="1"/>
+      <c r="V249" s="5"/>
       <c r="W249" s="7"/>
     </row>
     <row r="250" spans="1:23">
@@ -6528,7 +7001,7 @@
       <c r="S252" s="5"/>
       <c r="T252" s="5"/>
       <c r="U252" s="5"/>
-      <c r="V252" s="5"/>
+      <c r="V252" s="1"/>
       <c r="W252" s="7"/>
     </row>
     <row r="253" spans="1:23">
@@ -6550,7 +7023,7 @@
       <c r="S253" s="5"/>
       <c r="T253" s="5"/>
       <c r="U253" s="5"/>
-      <c r="V253" s="5"/>
+      <c r="V253" s="1"/>
       <c r="W253" s="7"/>
     </row>
     <row r="254" spans="1:23">
@@ -6572,7 +7045,7 @@
       <c r="S254" s="5"/>
       <c r="T254" s="5"/>
       <c r="U254" s="5"/>
-      <c r="V254" s="1"/>
+      <c r="V254" s="5"/>
       <c r="W254" s="7"/>
     </row>
     <row r="255" spans="1:23">
@@ -6594,7 +7067,7 @@
       <c r="S255" s="5"/>
       <c r="T255" s="5"/>
       <c r="U255" s="5"/>
-      <c r="V255" s="1"/>
+      <c r="V255" s="5"/>
       <c r="W255" s="7"/>
     </row>
     <row r="256" spans="1:23">
@@ -7144,7 +7617,7 @@
       <c r="S280" s="5"/>
       <c r="T280" s="5"/>
       <c r="U280" s="5"/>
-      <c r="V280" s="5"/>
+      <c r="V280" s="1"/>
       <c r="W280" s="7"/>
     </row>
     <row r="281" spans="2:23">
@@ -7166,7 +7639,7 @@
       <c r="S281" s="5"/>
       <c r="T281" s="5"/>
       <c r="U281" s="5"/>
-      <c r="V281" s="5"/>
+      <c r="V281" s="1"/>
       <c r="W281" s="7"/>
     </row>
     <row r="282" spans="2:23">
@@ -7188,7 +7661,7 @@
       <c r="S282" s="5"/>
       <c r="T282" s="5"/>
       <c r="U282" s="5"/>
-      <c r="V282" s="1"/>
+      <c r="V282" s="5"/>
       <c r="W282" s="7"/>
     </row>
     <row r="283" spans="2:23">
@@ -7210,7 +7683,7 @@
       <c r="S283" s="5"/>
       <c r="T283" s="5"/>
       <c r="U283" s="5"/>
-      <c r="V283" s="1"/>
+      <c r="V283" s="5"/>
       <c r="W283" s="7"/>
     </row>
     <row r="284" spans="2:23">
@@ -7232,7 +7705,7 @@
       <c r="S284" s="5"/>
       <c r="T284" s="5"/>
       <c r="U284" s="5"/>
-      <c r="V284" s="5"/>
+      <c r="V284" s="1"/>
       <c r="W284" s="7"/>
     </row>
     <row r="285" spans="2:23">
@@ -7276,7 +7749,7 @@
       <c r="S286" s="5"/>
       <c r="T286" s="5"/>
       <c r="U286" s="5"/>
-      <c r="V286" s="1"/>
+      <c r="V286" s="5"/>
       <c r="W286" s="7"/>
     </row>
     <row r="287" spans="2:23">
@@ -7804,7 +8277,7 @@
       <c r="S310" s="5"/>
       <c r="T310" s="5"/>
       <c r="U310" s="5"/>
-      <c r="V310" s="5"/>
+      <c r="V310" s="1"/>
       <c r="W310" s="7"/>
     </row>
     <row r="311" spans="2:23">
@@ -7826,7 +8299,7 @@
       <c r="S311" s="5"/>
       <c r="T311" s="5"/>
       <c r="U311" s="5"/>
-      <c r="V311" s="5"/>
+      <c r="V311" s="1"/>
       <c r="W311" s="7"/>
     </row>
     <row r="312" spans="2:23">
@@ -7914,7 +8387,7 @@
       <c r="S315" s="5"/>
       <c r="T315" s="5"/>
       <c r="U315" s="5"/>
-      <c r="V315" s="1"/>
+      <c r="V315" s="5"/>
       <c r="W315" s="7"/>
     </row>
     <row r="316" spans="2:23">
@@ -7936,7 +8409,7 @@
       <c r="S316" s="5"/>
       <c r="T316" s="5"/>
       <c r="U316" s="5"/>
-      <c r="V316" s="1"/>
+      <c r="V316" s="5"/>
       <c r="W316" s="7"/>
     </row>
     <row r="317" spans="2:23">
@@ -8002,7 +8475,7 @@
       <c r="S319" s="5"/>
       <c r="T319" s="5"/>
       <c r="U319" s="5"/>
-      <c r="V319" s="5"/>
+      <c r="V319" s="1"/>
       <c r="W319" s="7"/>
     </row>
     <row r="320" spans="2:23">
@@ -8024,7 +8497,7 @@
       <c r="S320" s="5"/>
       <c r="T320" s="5"/>
       <c r="U320" s="5"/>
-      <c r="V320" s="5"/>
+      <c r="V320" s="1"/>
       <c r="W320" s="7"/>
     </row>
     <row r="321" spans="2:23">
@@ -8046,7 +8519,7 @@
       <c r="S321" s="5"/>
       <c r="T321" s="5"/>
       <c r="U321" s="5"/>
-      <c r="V321" s="1"/>
+      <c r="V321" s="5"/>
       <c r="W321" s="7"/>
     </row>
     <row r="322" spans="2:23">
@@ -8068,7 +8541,7 @@
       <c r="S322" s="5"/>
       <c r="T322" s="5"/>
       <c r="U322" s="5"/>
-      <c r="V322" s="1"/>
+      <c r="V322" s="5"/>
       <c r="W322" s="7"/>
     </row>
     <row r="323" spans="2:23">
@@ -8090,7 +8563,7 @@
       <c r="S323" s="5"/>
       <c r="T323" s="5"/>
       <c r="U323" s="5"/>
-      <c r="V323" s="5"/>
+      <c r="V323" s="1"/>
       <c r="W323" s="7"/>
     </row>
     <row r="324" spans="2:23">
@@ -8112,7 +8585,7 @@
       <c r="S324" s="5"/>
       <c r="T324" s="5"/>
       <c r="U324" s="5"/>
-      <c r="V324" s="5"/>
+      <c r="V324" s="1"/>
       <c r="W324" s="7"/>
     </row>
     <row r="325" spans="2:23">
@@ -8134,7 +8607,7 @@
       <c r="S325" s="5"/>
       <c r="T325" s="5"/>
       <c r="U325" s="5"/>
-      <c r="V325" s="1"/>
+      <c r="V325" s="5"/>
       <c r="W325" s="7"/>
     </row>
     <row r="326" spans="2:23">
@@ -8156,7 +8629,7 @@
       <c r="S326" s="5"/>
       <c r="T326" s="5"/>
       <c r="U326" s="5"/>
-      <c r="V326" s="1"/>
+      <c r="V326" s="5"/>
       <c r="W326" s="7"/>
     </row>
     <row r="327" spans="2:23">
@@ -8486,7 +8959,7 @@
       <c r="S341" s="5"/>
       <c r="T341" s="5"/>
       <c r="U341" s="5"/>
-      <c r="V341" s="5"/>
+      <c r="V341" s="1"/>
       <c r="W341" s="7"/>
     </row>
     <row r="342" spans="2:23">
@@ -8508,7 +8981,7 @@
       <c r="S342" s="5"/>
       <c r="T342" s="5"/>
       <c r="U342" s="5"/>
-      <c r="V342" s="5"/>
+      <c r="V342" s="1"/>
       <c r="W342" s="7"/>
     </row>
     <row r="343" spans="2:23">
@@ -8530,7 +9003,7 @@
       <c r="S343" s="5"/>
       <c r="T343" s="5"/>
       <c r="U343" s="5"/>
-      <c r="V343" s="1"/>
+      <c r="V343" s="5"/>
       <c r="W343" s="7"/>
     </row>
     <row r="344" spans="2:23">
@@ -8552,7 +9025,7 @@
       <c r="S344" s="5"/>
       <c r="T344" s="5"/>
       <c r="U344" s="5"/>
-      <c r="V344" s="1"/>
+      <c r="V344" s="5"/>
       <c r="W344" s="7"/>
     </row>
     <row r="345" spans="2:23">
@@ -8662,7 +9135,7 @@
       <c r="S349" s="5"/>
       <c r="T349" s="5"/>
       <c r="U349" s="5"/>
-      <c r="V349" s="5"/>
+      <c r="V349" s="1"/>
       <c r="W349" s="7"/>
     </row>
     <row r="350" spans="2:23">
@@ -8684,7 +9157,7 @@
       <c r="S350" s="5"/>
       <c r="T350" s="5"/>
       <c r="U350" s="5"/>
-      <c r="V350" s="5"/>
+      <c r="V350" s="1"/>
       <c r="W350" s="7"/>
     </row>
     <row r="351" spans="2:23">
@@ -8706,7 +9179,7 @@
       <c r="S351" s="5"/>
       <c r="T351" s="5"/>
       <c r="U351" s="5"/>
-      <c r="V351" s="1"/>
+      <c r="V351" s="5"/>
       <c r="W351" s="7"/>
     </row>
     <row r="352" spans="2:23">
@@ -8728,7 +9201,7 @@
       <c r="S352" s="5"/>
       <c r="T352" s="5"/>
       <c r="U352" s="5"/>
-      <c r="V352" s="1"/>
+      <c r="V352" s="5"/>
       <c r="W352" s="7"/>
     </row>
     <row r="353" spans="2:23">
@@ -8750,7 +9223,7 @@
       <c r="S353" s="5"/>
       <c r="T353" s="5"/>
       <c r="U353" s="5"/>
-      <c r="V353" s="5"/>
+      <c r="V353" s="1"/>
       <c r="W353" s="7"/>
     </row>
     <row r="354" spans="2:23">
@@ -8794,7 +9267,7 @@
       <c r="S355" s="5"/>
       <c r="T355" s="5"/>
       <c r="U355" s="5"/>
-      <c r="V355" s="1"/>
+      <c r="V355" s="5"/>
       <c r="W355" s="7"/>
     </row>
     <row r="356" spans="2:23">
@@ -9234,7 +9707,7 @@
       <c r="S375" s="5"/>
       <c r="T375" s="5"/>
       <c r="U375" s="5"/>
-      <c r="V375" s="5"/>
+      <c r="V375" s="1"/>
       <c r="W375" s="7"/>
     </row>
     <row r="376" spans="2:23">
@@ -9256,7 +9729,7 @@
       <c r="S376" s="5"/>
       <c r="T376" s="5"/>
       <c r="U376" s="5"/>
-      <c r="V376" s="5"/>
+      <c r="V376" s="1"/>
       <c r="W376" s="7"/>
     </row>
     <row r="377" spans="2:23">
@@ -9344,7 +9817,7 @@
       <c r="S380" s="5"/>
       <c r="T380" s="5"/>
       <c r="U380" s="5"/>
-      <c r="V380" s="1"/>
+      <c r="V380" s="5"/>
       <c r="W380" s="7"/>
     </row>
     <row r="381" spans="2:23">
@@ -9366,7 +9839,7 @@
       <c r="S381" s="5"/>
       <c r="T381" s="5"/>
       <c r="U381" s="5"/>
-      <c r="V381" s="1"/>
+      <c r="V381" s="5"/>
       <c r="W381" s="7"/>
     </row>
     <row r="382" spans="2:23">
@@ -9432,7 +9905,7 @@
       <c r="S384" s="5"/>
       <c r="T384" s="5"/>
       <c r="U384" s="5"/>
-      <c r="V384" s="5"/>
+      <c r="V384" s="1"/>
       <c r="W384" s="7"/>
     </row>
     <row r="385" spans="2:23">
@@ -9454,7 +9927,7 @@
       <c r="S385" s="5"/>
       <c r="T385" s="5"/>
       <c r="U385" s="5"/>
-      <c r="V385" s="5"/>
+      <c r="V385" s="1"/>
       <c r="W385" s="7"/>
     </row>
     <row r="386" spans="2:23">
@@ -9476,7 +9949,7 @@
       <c r="S386" s="5"/>
       <c r="T386" s="5"/>
       <c r="U386" s="5"/>
-      <c r="V386" s="1"/>
+      <c r="V386" s="5"/>
       <c r="W386" s="7"/>
     </row>
     <row r="387" spans="2:23">
@@ -9498,7 +9971,7 @@
       <c r="S387" s="5"/>
       <c r="T387" s="5"/>
       <c r="U387" s="5"/>
-      <c r="V387" s="1"/>
+      <c r="V387" s="5"/>
       <c r="W387" s="7"/>
     </row>
     <row r="388" spans="2:23">
@@ -9520,7 +9993,7 @@
       <c r="S388" s="5"/>
       <c r="T388" s="5"/>
       <c r="U388" s="5"/>
-      <c r="V388" s="5"/>
+      <c r="V388" s="1"/>
       <c r="W388" s="7"/>
     </row>
     <row r="389" spans="2:23">
@@ -9542,7 +10015,7 @@
       <c r="S389" s="5"/>
       <c r="T389" s="5"/>
       <c r="U389" s="5"/>
-      <c r="V389" s="5"/>
+      <c r="V389" s="1"/>
       <c r="W389" s="7"/>
     </row>
     <row r="390" spans="2:23">
@@ -9564,7 +10037,7 @@
       <c r="S390" s="5"/>
       <c r="T390" s="5"/>
       <c r="U390" s="5"/>
-      <c r="V390" s="1"/>
+      <c r="V390" s="5"/>
       <c r="W390" s="7"/>
     </row>
     <row r="391" spans="2:23">
@@ -9586,7 +10059,7 @@
       <c r="S391" s="5"/>
       <c r="T391" s="5"/>
       <c r="U391" s="5"/>
-      <c r="V391" s="1"/>
+      <c r="V391" s="5"/>
       <c r="W391" s="7"/>
     </row>
     <row r="392" spans="2:23">
@@ -9916,10 +10389,11 @@
       <c r="S406" s="5"/>
       <c r="T406" s="5"/>
       <c r="U406" s="5"/>
-      <c r="V406" s="5"/>
+      <c r="V406" s="1"/>
       <c r="W406" s="7"/>
     </row>
     <row r="407" spans="1:23">
+      <c r="A407" s="8"/>
       <c r="B407" s="5"/>
       <c r="C407" s="5"/>
       <c r="D407" s="5"/>
@@ -9938,7 +10412,7 @@
       <c r="S407" s="5"/>
       <c r="T407" s="5"/>
       <c r="U407" s="5"/>
-      <c r="V407" s="5"/>
+      <c r="V407" s="1"/>
       <c r="W407" s="7"/>
     </row>
     <row r="408" spans="1:23">
@@ -9960,11 +10434,10 @@
       <c r="S408" s="5"/>
       <c r="T408" s="5"/>
       <c r="U408" s="5"/>
-      <c r="V408" s="1"/>
+      <c r="V408" s="5"/>
       <c r="W408" s="7"/>
     </row>
     <row r="409" spans="1:23">
-      <c r="A409" s="8"/>
       <c r="B409" s="5"/>
       <c r="C409" s="5"/>
       <c r="D409" s="5"/>
@@ -9983,7 +10456,7 @@
       <c r="S409" s="5"/>
       <c r="T409" s="5"/>
       <c r="U409" s="5"/>
-      <c r="V409" s="1"/>
+      <c r="V409" s="5"/>
       <c r="W409" s="7"/>
     </row>
     <row r="410" spans="1:23">
@@ -10075,6 +10548,7 @@
       <c r="W413" s="7"/>
     </row>
     <row r="414" spans="1:23">
+      <c r="A414" s="3"/>
       <c r="B414" s="5"/>
       <c r="C414" s="5"/>
       <c r="D414" s="5"/>
@@ -10093,10 +10567,11 @@
       <c r="S414" s="5"/>
       <c r="T414" s="5"/>
       <c r="U414" s="5"/>
-      <c r="V414" s="5"/>
+      <c r="V414" s="1"/>
       <c r="W414" s="7"/>
     </row>
     <row r="415" spans="1:23">
+      <c r="A415" s="8"/>
       <c r="B415" s="5"/>
       <c r="C415" s="5"/>
       <c r="D415" s="5"/>
@@ -10115,11 +10590,10 @@
       <c r="S415" s="5"/>
       <c r="T415" s="5"/>
       <c r="U415" s="5"/>
-      <c r="V415" s="5"/>
+      <c r="V415" s="1"/>
       <c r="W415" s="7"/>
     </row>
     <row r="416" spans="1:23">
-      <c r="A416" s="3"/>
       <c r="B416" s="5"/>
       <c r="C416" s="5"/>
       <c r="D416" s="5"/>
@@ -10138,11 +10612,10 @@
       <c r="S416" s="5"/>
       <c r="T416" s="5"/>
       <c r="U416" s="5"/>
-      <c r="V416" s="1"/>
+      <c r="V416" s="5"/>
       <c r="W416" s="7"/>
     </row>
-    <row r="417" spans="1:23">
-      <c r="A417" s="8"/>
+    <row r="417" spans="2:23">
       <c r="B417" s="5"/>
       <c r="C417" s="5"/>
       <c r="D417" s="5"/>
@@ -10161,10 +10634,10 @@
       <c r="S417" s="5"/>
       <c r="T417" s="5"/>
       <c r="U417" s="5"/>
-      <c r="V417" s="1"/>
+      <c r="V417" s="5"/>
       <c r="W417" s="7"/>
     </row>
-    <row r="418" spans="1:23">
+    <row r="418" spans="2:23">
       <c r="B418" s="5"/>
       <c r="C418" s="5"/>
       <c r="D418" s="5"/>
@@ -10183,52 +10656,8 @@
       <c r="S418" s="5"/>
       <c r="T418" s="5"/>
       <c r="U418" s="5"/>
-      <c r="V418" s="5"/>
+      <c r="V418" s="1"/>
       <c r="W418" s="7"/>
-    </row>
-    <row r="419" spans="1:23">
-      <c r="B419" s="5"/>
-      <c r="C419" s="5"/>
-      <c r="D419" s="5"/>
-      <c r="E419" s="5"/>
-      <c r="H419" s="5"/>
-      <c r="I419" s="5"/>
-      <c r="J419" s="5"/>
-      <c r="K419" s="5"/>
-      <c r="L419" s="5"/>
-      <c r="M419" s="6"/>
-      <c r="N419" s="5"/>
-      <c r="O419" s="5"/>
-      <c r="P419" s="5"/>
-      <c r="Q419" s="5"/>
-      <c r="R419" s="5"/>
-      <c r="S419" s="5"/>
-      <c r="T419" s="5"/>
-      <c r="U419" s="5"/>
-      <c r="V419" s="5"/>
-      <c r="W419" s="7"/>
-    </row>
-    <row r="420" spans="1:23">
-      <c r="B420" s="5"/>
-      <c r="C420" s="5"/>
-      <c r="D420" s="5"/>
-      <c r="E420" s="5"/>
-      <c r="H420" s="5"/>
-      <c r="I420" s="5"/>
-      <c r="J420" s="5"/>
-      <c r="K420" s="5"/>
-      <c r="L420" s="5"/>
-      <c r="M420" s="6"/>
-      <c r="N420" s="5"/>
-      <c r="O420" s="5"/>
-      <c r="P420" s="5"/>
-      <c r="Q420" s="5"/>
-      <c r="R420" s="5"/>
-      <c r="S420" s="5"/>
-      <c r="T420" s="5"/>
-      <c r="U420" s="5"/>
-      <c r="V420" s="1"/>
-      <c r="W420" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>